<commit_message>
Some changes I don't remenber doing
</commit_message>
<xml_diff>
--- a/Projeto/Relatorios Contribuição/ContribuicaoIndividual - P2.xlsx
+++ b/Projeto/Relatorios Contribuição/ContribuicaoIndividual - P2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Web\Rolling-Tetris-Web\Projeto\Relatorios Contribuição\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5A7C9B-A8D4-42A0-8047-D96EA7C52749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F881D678-AF60-47F1-A144-8936EA514671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="1065" windowWidth="20640" windowHeight="11760" xr2:uid="{8AD44023-9501-48E1-8BFC-2E44CC22AE8A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Relatório de Contribuição Individual</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>Projeto Final - Rolling Tetris - Parte 2</t>
+  </si>
+  <si>
+    <t>Organizou o grupo, implementou todo jogo e tabelas</t>
+  </si>
+  <si>
+    <t>cuidou da página login</t>
+  </si>
+  <si>
+    <t>cuidou da página registrar</t>
+  </si>
+  <si>
+    <t>cuidou da página de alterar informações</t>
   </si>
 </sst>
 </file>
@@ -835,7 +847,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,9 +961,11 @@
         <v>231396</v>
       </c>
       <c r="D9" s="24">
-        <v>0.25</v>
-      </c>
-      <c r="E9" s="27"/>
+        <v>0.36</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="F9" s="31">
         <f>IF(D9="","",IF($A$18="",ROUND(MIN(MIN(10,$F$6+1),COUNTA($D$9:$D$13)*$F$6*D9),1),"Erro"))</f>
         <v>10</v>
@@ -968,12 +982,14 @@
         <v>240147</v>
       </c>
       <c r="D10" s="24">
-        <v>0.25</v>
-      </c>
-      <c r="E10" s="23"/>
+        <v>0.215</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>31</v>
+      </c>
       <c r="F10" s="31">
         <f t="shared" ref="F10:F13" si="0">IF(D10="","",IF($A$18="",ROUND(MIN(MIN(10,$F$6+1),COUNTA($D$9:$D$13)*$F$6*D10),1),"Erro"))</f>
-        <v>10</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,12 +1003,14 @@
         <v>245517</v>
       </c>
       <c r="D11" s="24">
-        <v>0.25</v>
-      </c>
-      <c r="E11" s="23"/>
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="F11" s="31">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1006,12 +1024,14 @@
         <v>173381</v>
       </c>
       <c r="D12" s="24">
-        <v>0.25</v>
-      </c>
-      <c r="E12" s="23"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F12" s="31">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,7 +1078,7 @@
       <c r="E16" s="38"/>
       <c r="F16" s="6">
         <f ca="1">NOW()</f>
-        <v>44124.177673032405</v>
+        <v>44159.795660532407</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1310,21 +1330,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010027B1B795F3ACD74191B7284862A64588" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="9ae5dfd6e757cdf140f76020e29a6e0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="de106b6a-02b6-4774-b219-e71fbb5cc1ce" xmlns:ns4="5feea0e9-8f6d-471c-b84e-b049251fc55f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d30e59c414edc37baddb95c666cd0950" ns3:_="" ns4:_="">
     <xsd:import namespace="de106b6a-02b6-4774-b219-e71fbb5cc1ce"/>
@@ -1547,32 +1552,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0537F2A3-82D8-4D11-AF44-B60EFF661ED7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5feea0e9-8f6d-471c-b84e-b049251fc55f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="de106b6a-02b6-4774-b219-e71fbb5cc1ce"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDB3412-F176-463C-9CD3-ADF26C83D016}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{674BDE44-CA73-45BE-9BAA-FE3EA527B3F3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1589,4 +1584,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDB3412-F176-463C-9CD3-ADF26C83D016}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0537F2A3-82D8-4D11-AF44-B60EFF661ED7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5feea0e9-8f6d-471c-b84e-b049251fc55f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="de106b6a-02b6-4774-b219-e71fbb5cc1ce"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>